<commit_message>
Minor fix for friction
</commit_message>
<xml_diff>
--- a/Input/NewData_Zahra_3D.xlsx
+++ b/Input/NewData_Zahra_3D.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univoftulsa-my.sharepoint.com/personal/elh1873_utulsa_edu/Documents/Shell - MOD1/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univoftulsa-my.sharepoint.com/personal/elh1873_utulsa_edu/Documents/PHD/Models/Dynamic-Torque-and-Drag-Model/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="839" documentId="114_{9D85A293-3D7E-45E3-94E2-3BBAC28D502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE3AD28D-D395-43C7-AB3D-A906D1ED4178}"/>
+  <xr:revisionPtr revIDLastSave="842" documentId="114_{9D85A293-3D7E-45E3-94E2-3BBAC28D502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9F6155A-BBB1-4414-B734-BEE3AAE7DC6C}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="3270" windowWidth="21600" windowHeight="11295" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="3270" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SURVEY" sheetId="5" r:id="rId1"/>
@@ -734,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB77188-32FA-43EE-BD2E-FA6085E2DDB4}">
   <dimension ref="A1:D687"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5004,7 +5004,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5064,7 +5064,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -5250,7 +5250,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5271,7 +5271,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="6">
-        <v>-50</v>
+        <v>-171</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5279,7 +5279,7 @@
         <v>76</v>
       </c>
       <c r="B3" s="6">
-        <v>-50</v>
+        <v>-171</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -5403,7 +5403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B63BE9C-B52F-42E9-B3E2-E06B21071682}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New input & solver
</commit_message>
<xml_diff>
--- a/Input/NewData_Zahra_3D.xlsx
+++ b/Input/NewData_Zahra_3D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univoftulsa-my.sharepoint.com/personal/elh1873_utulsa_edu/Documents/PHD/Models/Dynamic-Torque-and-Drag-Model/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="842" documentId="114_{9D85A293-3D7E-45E3-94E2-3BBAC28D502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9F6155A-BBB1-4414-B734-BEE3AAE7DC6C}"/>
+  <xr:revisionPtr revIDLastSave="870" documentId="114_{9D85A293-3D7E-45E3-94E2-3BBAC28D502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26792D64-747F-4193-9F68-27E04795701F}"/>
   <bookViews>
-    <workbookView xWindow="3390" yWindow="3270" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SURVEY" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
   <si>
     <t>BHA Type</t>
   </si>
@@ -142,9 +142,6 @@
     <t>cP</t>
   </si>
   <si>
-    <t>lbf/100ft^2</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
@@ -193,12 +190,6 @@
     <t>a4</t>
   </si>
   <si>
-    <t>Top Drive RPM Magnitude 1 (RPM)</t>
-  </si>
-  <si>
-    <t>Top Drive RPM Magnitude 2 (RPM)</t>
-  </si>
-  <si>
     <t>b1</t>
   </si>
   <si>
@@ -271,12 +262,6 @@
     <t>Collars</t>
   </si>
   <si>
-    <t>Top Drive Axial Velocity Magnitude 1 (ft/min)</t>
-  </si>
-  <si>
-    <t>Top Drive Axial Velocity Magnitude 2 (ft/min)</t>
-  </si>
-  <si>
     <t>Shear Modulus</t>
   </si>
   <si>
@@ -284,6 +269,36 @@
   </si>
   <si>
     <t>GPM</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Top Drive ROP 1</t>
+  </si>
+  <si>
+    <t>Top Drive ROP 2</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>Top Drive RPM 1</t>
+  </si>
+  <si>
+    <t>Top Drive RPM 2</t>
+  </si>
+  <si>
+    <t>Top Drive Weight</t>
+  </si>
+  <si>
+    <t>ft/min</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>lbf</t>
   </si>
 </sst>
 </file>
@@ -374,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -425,6 +440,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB77188-32FA-43EE-BD2E-FA6085E2DDB4}">
   <dimension ref="A1:D687"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3819,7 +3835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -3840,7 +3856,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
@@ -3875,7 +3891,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -3916,7 +3932,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -3998,7 +4014,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -5001,10 +5017,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E72B133-B881-4CF1-A552-650940017511}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5023,12 +5039,12 @@
         <v>27</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1">
         <v>12</v>
@@ -5039,7 +5055,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1">
         <v>65.5</v>
@@ -5064,63 +5080,72 @@
         <v>30</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1">
         <f>15000</f>
         <v>15000</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G12" s="1"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5133,7 +5158,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5142,6 +5167,7 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5152,84 +5178,85 @@
         <v>27</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1">
         <v>8.5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1">
         <v>14500</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B4" s="6">
         <v>60808000000</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="9">
-        <v>4320000000</v>
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>206842498560</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B6" s="14">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1">
         <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B8" s="1">
         <v>200</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5247,7 +5274,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EF5AC9-A478-4C3E-B910-9FDDED31D199}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -5258,140 +5285,187 @@
     <col min="1" max="1" width="41.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B2" s="6">
         <v>-171</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" s="6">
         <v>-171</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="6">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="6">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="6">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="6">
+        <v>63</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="6">
+        <v>66</v>
+      </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="6">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="6">
+        <v>33</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="6">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="6">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="6">
         <v>66</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="6">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="6">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="6">
-        <v>66</v>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -5404,31 +5478,34 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
-        <v>33</v>
+      <c r="C1" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>79</v>
+      <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5460,34 +5537,34 @@
         <v>27</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1">
         <v>1500</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B3" s="1">
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1">
         <v>120</v>

</xml_diff>